<commit_message>
read more sheet in one xlsx
</commit_message>
<xml_diff>
--- a/Xlsx-Project/public/test.xlsx
+++ b/Xlsx-Project/public/test.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git_project\nodejs_demo\Xlsx\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git_project\nodejs_demo\Xlsx-Project\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7062ECC1-1F6C-40FA-A095-4891D2A87370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EE0E23-1FF1-48B7-A8BC-276E51355FBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="tarot" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -77,6 +78,94 @@
   <si>
     <t>guangdong</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>star</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>power</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{type:1, value:100}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>quality</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{type:1, value:101}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:102}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:103}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:104}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:105}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:106}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:107}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:108}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:109}}</t>
+  </si>
+  <si>
+    <t>{{type:1, value:110}}</t>
+  </si>
+  <si>
+    <t>这是品质1的塔罗牌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>这是品质2的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质3的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质4的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质5的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质6的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质7的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质8的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质9的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质10的塔罗牌</t>
+  </si>
+  <si>
+    <t>这是品质11的塔罗牌</t>
   </si>
 </sst>
 </file>
@@ -442,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -531,4 +620,265 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1D672C-EE2A-4E3B-856A-599F8BE7202A}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1300</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1600</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1700</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1800</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2100</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>910001</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2200</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>